<commit_message>
auto fix row data
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
@@ -384,10 +384,49 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -404,45 +443,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -759,7 +759,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:P12"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,48 +778,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
     </row>
     <row r="3" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
@@ -851,7 +851,7 @@
         <v>19</v>
       </c>
       <c r="M3" s="25"/>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="27" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="25" t="s">
@@ -860,7 +860,7 @@
       <c r="P3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="26" t="s">
         <v>5</v>
       </c>
       <c r="R3" s="25" t="s">
@@ -901,10 +901,10 @@
       <c r="M4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="42"/>
+      <c r="N4" s="28"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
-      <c r="Q4" s="31"/>
+      <c r="Q4" s="26"/>
       <c r="R4" s="25"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -928,24 +928,24 @@
       <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="21"/>
     </row>
@@ -982,18 +982,18 @@
         <v>20</v>
       </c>
       <c r="E8" s="25"/>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="33" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="33" t="s">
+      <c r="I8" s="33"/>
+      <c r="J8" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="39"/>
+      <c r="K8" s="38"/>
       <c r="L8" s="25" t="s">
         <v>24</v>
       </c>
@@ -1001,11 +1001,11 @@
         <v>4</v>
       </c>
       <c r="N8" s="25"/>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="31" t="s">
+      <c r="P8" s="35"/>
+      <c r="Q8" s="26" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="25" t="s">
@@ -1043,35 +1043,31 @@
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="32"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="30"/>
       <c r="R9" s="25"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28">
-        <v>14355000</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="23">
-        <v>2153250</v>
-      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="23"/>
       <c r="R10" s="22"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1087,54 +1083,54 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="27"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="40"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="20"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="21"/>
     </row>
@@ -1186,6 +1182,25 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A12:P12"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:P10"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -1201,25 +1216,6 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A12:P12"/>
-    <mergeCell ref="A13:P13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update BSTTCS and TTCS
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
@@ -74,27 +74,15 @@
     <t>Bs_TTN</t>
   </si>
   <si>
-    <t>Bs_Sapo</t>
-  </si>
-  <si>
     <t>K/Thinh</t>
   </si>
   <si>
     <t>T/File</t>
   </si>
   <si>
-    <t>Bt Duyet</t>
-  </si>
-  <si>
     <t>DCT</t>
   </si>
   <si>
-    <t>KTD</t>
-  </si>
-  <si>
-    <t>TCT</t>
-  </si>
-  <si>
     <t>KT_TH</t>
   </si>
   <si>
@@ -114,6 +102,18 @@
   </si>
   <si>
     <t>Ban biên tập 15%</t>
+  </si>
+  <si>
+    <t>Bs_Sapo/ Tỉnh</t>
+  </si>
+  <si>
+    <t>Bt Duyet Sa/Tối</t>
+  </si>
+  <si>
+    <t>KTD Sa/Tối</t>
+  </si>
+  <si>
+    <t>TCT Sa</t>
   </si>
 </sst>
 </file>
@@ -440,13 +440,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -805,7 +805,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" activeCellId="5" sqref="E1:E1048576 G1:G1048576 I1:I1048576 K1:K1048576 M1:M1048576 O1:O1048576"/>
+      <selection activeCell="H8" sqref="H8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -855,7 +855,7 @@
     </row>
     <row r="2" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -875,7 +875,7 @@
       <c r="Q2" s="49"/>
       <c r="R2" s="49"/>
     </row>
-    <row r="3" spans="1:18" s="12" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
@@ -890,29 +890,29 @@
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="40"/>
       <c r="J3" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="40"/>
       <c r="L3" s="40" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="M3" s="40"/>
       <c r="N3" s="47" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="O3" s="30" t="s">
         <v>4</v>
       </c>
       <c r="P3" s="30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="Q3" s="36" t="s">
         <v>5</v>
@@ -961,7 +961,7 @@
       <c r="Q4" s="36"/>
       <c r="R4" s="30"/>
     </row>
-    <row r="5" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1022,7 +1022,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="20"/>
     </row>
-    <row r="8" spans="1:18" s="12" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="12" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>1</v>
       </c>
@@ -1033,30 +1033,30 @@
         <v>3</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="40"/>
       <c r="F8" s="38" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G8" s="39"/>
       <c r="H8" s="38" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I8" s="39"/>
       <c r="J8" s="38" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K8" s="45"/>
       <c r="L8" s="30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M8" s="30" t="s">
         <v>4</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P8" s="42"/>
       <c r="Q8" s="36" t="s">
@@ -1105,7 +1105,7 @@
     <row r="10" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33"/>
@@ -1124,7 +1124,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="13" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -1188,13 +1188,13 @@
       <c r="Q13" s="27"/>
       <c r="R13" s="28"/>
     </row>
-    <row r="14" spans="1:18" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="11" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q14" s="21"/>
       <c r="R14" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1211,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
resize columns width in import form, resize column height in report
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
@@ -427,10 +427,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -447,48 +489,6 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -805,10 +805,10 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:I8"/>
+      <selection activeCell="P3" sqref="P3:P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
@@ -832,99 +832,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-    </row>
-    <row r="3" spans="1:18" s="12" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+    </row>
+    <row r="3" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40" t="s">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40" t="s">
+      <c r="K3" s="30"/>
+      <c r="L3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="47" t="s">
+      <c r="M3" s="30"/>
+      <c r="N3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+    <row r="4" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
@@ -955,13 +955,13 @@
       <c r="M4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="48"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="30"/>
-    </row>
-    <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="34"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="31"/>
+    </row>
+    <row r="5" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -981,29 +981,29 @@
       <c r="Q5" s="19"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="28"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1022,20 +1022,20 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="20"/>
     </row>
-    <row r="8" spans="1:18" s="12" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="38" t="s">
         <v>28</v>
       </c>
@@ -1047,29 +1047,29 @@
       <c r="J8" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="45"/>
-      <c r="L8" s="30" t="s">
+      <c r="K8" s="44"/>
+      <c r="L8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="30"/>
-      <c r="O8" s="41" t="s">
+      <c r="N8" s="31"/>
+      <c r="O8" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="36" t="s">
+      <c r="P8" s="41"/>
+      <c r="Q8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
+    <row r="9" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1094,37 +1094,37 @@
       <c r="K9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="30"/>
-    </row>
-    <row r="10" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="31"/>
+    </row>
+    <row r="10" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="35"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="49"/>
       <c r="Q10" s="25"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1137,64 +1137,64 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="32"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="46"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="24"/>
     </row>
-    <row r="12" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
       <c r="Q12" s="27"/>
       <c r="R12" s="28"/>
     </row>
-    <row r="13" spans="1:18" s="26" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
       <c r="Q13" s="27"/>
       <c r="R13" s="28"/>
     </row>
-    <row r="14" spans="1:18" s="11" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q14" s="21"/>
       <c r="R14" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="32.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1211,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="17" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>11</v>
       </c>
@@ -1227,6 +1227,25 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A12:P12"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:P10"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -1242,25 +1261,6 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A12:P12"/>
-    <mergeCell ref="A13:P13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update templateBSTTCS and not increase percent if point is negative
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
+++ b/ATV_Allowance/Templates/TemplateBSTTCS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -114,6 +114,10 @@
   </si>
   <si>
     <t>TCT Sa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khối hậu kỳ
+</t>
   </si>
 </sst>
 </file>
@@ -357,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -369,14 +373,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -406,7 +408,6 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -427,18 +428,60 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -448,47 +491,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -804,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:P4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -813,155 +824,155 @@
     <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="6" style="10" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="6" style="8" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" style="8" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" style="23" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="20" customWidth="1"/>
     <col min="18" max="18" width="14.5703125" style="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:18" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-    </row>
-    <row r="3" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+    </row>
+    <row r="3" spans="1:18" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="37"/>
+      <c r="J3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="37"/>
+      <c r="L3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="30"/>
-      <c r="N3" s="33" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="31" t="s">
+      <c r="O3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="31" t="s">
+      <c r="R3" s="27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="13" t="s">
+    <row r="4" spans="1:18" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="34"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="31"/>
-    </row>
-    <row r="5" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="45"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="27"/>
+    </row>
+    <row r="5" spans="1:18" s="23" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -978,154 +989,156 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="24"/>
-    </row>
-    <row r="6" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="Q5" s="17"/>
+      <c r="R5" s="21"/>
+    </row>
+    <row r="6" spans="1:18" s="23" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="28"/>
-    </row>
-    <row r="7" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="20"/>
-    </row>
-    <row r="8" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="25"/>
+    </row>
+    <row r="7" spans="1:18" s="50" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="47"/>
+      <c r="B7" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="49"/>
+    </row>
+    <row r="8" spans="1:18" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="38" t="s">
+      <c r="E8" s="37"/>
+      <c r="F8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="38" t="s">
+      <c r="G8" s="36"/>
+      <c r="H8" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="38" t="s">
+      <c r="I8" s="36"/>
+      <c r="J8" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="31" t="s">
+      <c r="K8" s="42"/>
+      <c r="L8" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="31"/>
-      <c r="O8" s="40" t="s">
+      <c r="N8" s="27"/>
+      <c r="O8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="32" t="s">
+      <c r="P8" s="39"/>
+      <c r="Q8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="31" t="s">
+      <c r="R8" s="27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="13" t="s">
+    <row r="9" spans="1:18" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="31"/>
-    </row>
-    <row r="10" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="45" t="s">
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="27"/>
+    </row>
+    <row r="10" spans="1:18" s="23" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="21"/>
+    </row>
+    <row r="11" spans="1:18" s="23" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
@@ -1137,60 +1150,60 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="24"/>
-    </row>
-    <row r="12" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="M11" s="28"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="21"/>
+    </row>
+    <row r="12" spans="1:18" s="23" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="28"/>
-    </row>
-    <row r="13" spans="1:18" s="26" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="25"/>
+    </row>
+    <row r="13" spans="1:18" s="23" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="28"/>
-    </row>
-    <row r="14" spans="1:18" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q14" s="21"/>
-      <c r="R14" s="15" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="18"/>
+      <c r="R14" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1206,46 +1219,27 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="16" t="s">
+      <c r="Q15" s="19"/>
+      <c r="R15" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="17" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
+    <row r="16" spans="1:18" s="15" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q16" s="18" t="s">
+      <c r="Q16" s="16" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A12:P12"/>
-    <mergeCell ref="A13:P13"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:P10"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
+  <mergeCells count="35">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -1261,6 +1255,26 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="R3:R4"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="O8:P9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A12:P12"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>